<commit_message>
feat: initialize multi-platform Flutter project with core features and architecture.
</commit_message>
<xml_diff>
--- a/Inv.xlsx
+++ b/Inv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dinuk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dinuk\Investment-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292CCF50-7C7E-4E24-89D7-9ADF8539F95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510E05E8-95D1-4372-8D7F-5DBE454E69C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{72DAA1D2-9D2F-48D1-9E66-1118664FF5BB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="79">
   <si>
     <t>Where</t>
   </si>
@@ -255,13 +255,34 @@
   </si>
   <si>
     <t>Matured</t>
+  </si>
+  <si>
+    <t>Loan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount </t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>HNB Account Creation</t>
+  </si>
+  <si>
+    <t>Loan Pay for 2 months(March, April)</t>
+  </si>
+  <si>
+    <t>HNB Transferred</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +300,13 @@
     <font>
       <sz val="22"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -379,10 +407,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -448,6 +477,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -469,11 +501,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -806,16 +839,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9F2A58-A0C2-4CFD-A939-076BF73C65B0}">
-  <dimension ref="A1:BCY44"/>
+  <dimension ref="A1:BCY51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="75" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="3" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="24.109375" customWidth="1"/>
     <col min="5" max="5" width="25.44140625" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="3" customWidth="1"/>
@@ -830,18 +864,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1455" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="7"/>
       <c r="L1" s="23"/>
     </row>
@@ -909,35 +943,35 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:1455" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35">
         <v>415000</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="35">
         <v>6</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="36">
         <v>1</v>
       </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="42">
+      <c r="G4" s="36"/>
+      <c r="H4" s="35">
         <f>((D4*E4)*F4)/(12*100)</f>
         <v>2075</v>
       </c>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42" t="s">
+      <c r="I4" s="35"/>
+      <c r="J4" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="44">
+      <c r="K4" s="37">
         <v>46791</v>
       </c>
-      <c r="L4" s="42" t="s">
+      <c r="L4" s="35" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1037,22 +1071,22 @@
       <c r="K8" s="30"/>
     </row>
     <row r="10" spans="1:1455" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="37"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="40"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
     </row>
     <row r="11" spans="1:1455" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
@@ -2942,12 +2976,12 @@
       <c r="F29" s="30"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -3182,6 +3216,53 @@
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="45">
+        <v>9900000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="45">
+        <v>5000</v>
+      </c>
+      <c r="C48" s="46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="45">
+        <v>54000</v>
+      </c>
+      <c r="C49" s="47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="45">
+        <v>940000</v>
+      </c>
+      <c r="C50" s="47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="45"/>
+      <c r="C51" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>